<commit_message>
Added logs into Asserts, fixed bugs
</commit_message>
<xml_diff>
--- a/oms_test_framework_dotNET/Resources/DataProvider/UserSearchTest.xlsx
+++ b/oms_test_framework_dotNET/Resources/DataProvider/UserSearchTest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kvita\Desktop\SoftServe\Projects.dotNet\oms_test_framework_dotNET\oms_test_framework_dotNET\Resources\DataProvider\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoftServe\Projects\oms_test_framework_dotNET\oms_test_framework_dotNET\Resources\DataProvider\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="7032" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13020" windowHeight="7032"/>
   </bookViews>
   <sheets>
     <sheet name="AllColumnsFilter" sheetId="1" r:id="rId1"/>
@@ -682,48 +682,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% – Акцентування1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% – Акцентування2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% – Акцентування3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% – Акцентування4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% – Акцентування5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% – Акцентування6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% – Акцентування1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% – Акцентування2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% – Акцентування3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% – Акцентування4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% – Акцентування5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% – Акцентування6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% – Акцентування1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% – Акцентування2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% – Акцентування3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% – Акцентування4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% – Акцентування5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% – Акцентування6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Акцентування1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Акцентування2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Акцентування3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Акцентування4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Акцентування5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Акцентування6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ввід" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Гарний" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Заголовок 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Заголовок 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Заголовок 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Заголовок 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
-    <cellStyle name="Зв'язана клітинка" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Контрольна клітинка" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Назва" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральний" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обчислення" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Підсумок" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Поганий" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Примітка" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Результат" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Текст попередження" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Текст пояснення" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -741,7 +741,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Офіс">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -779,7 +779,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Офіс">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -851,7 +851,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Офіс">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1051,7 +1051,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>